<commit_message>
EME - le démarchage téléphonique
</commit_message>
<xml_diff>
--- a/recherche_stage/Prospection stage IFOCOP.xlsx
+++ b/recherche_stage/Prospection stage IFOCOP.xlsx
@@ -5,14 +5,16 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chmoxster/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chmoxster/Dropbox/IFOCOP - les cours/recherche_stage/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
+    <sheet name="agences web" sheetId="3" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="94">
   <si>
     <t>Entreprise</t>
   </si>
@@ -201,15 +203,139 @@
   </si>
   <si>
     <t>Uber</t>
+  </si>
+  <si>
+    <t>Oui Web</t>
+  </si>
+  <si>
+    <t>http://www.oui-web.fr</t>
+  </si>
+  <si>
+    <t>tel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 61 00 79 70 </t>
+  </si>
+  <si>
+    <t>http://www.peoleo.com</t>
+  </si>
+  <si>
+    <t>Peo Leo</t>
+  </si>
+  <si>
+    <t>01 43 29 73 73</t>
+  </si>
+  <si>
+    <t>Net First</t>
+  </si>
+  <si>
+    <t>http//www.netfirst.fr</t>
+  </si>
+  <si>
+    <t>01 85 09 26 02</t>
+  </si>
+  <si>
+    <t>http://www.orixa-media.com/?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orixia Media </t>
+  </si>
+  <si>
+    <t>01 80 96 85 42</t>
+  </si>
+  <si>
+    <t>Declicnet</t>
+  </si>
+  <si>
+    <t>http://www.declicweb.fr/</t>
+  </si>
+  <si>
+    <t>06 52 34 15 53</t>
+  </si>
+  <si>
+    <t>http://www.buddyweb.fr/</t>
+  </si>
+  <si>
+    <t>BuddyWeb</t>
+  </si>
+  <si>
+    <t>09 84 08 93 72</t>
+  </si>
+  <si>
+    <t>Radis Noir</t>
+  </si>
+  <si>
+    <t>http://www.radisnoir.com/</t>
+  </si>
+  <si>
+    <t>0970 466 036</t>
+  </si>
+  <si>
+    <t>http://www.netemedia.fr/</t>
+  </si>
+  <si>
+    <t>Netemedia</t>
+  </si>
+  <si>
+    <t>Sismeo</t>
+  </si>
+  <si>
+    <t>http://www.sismeo.com/</t>
+  </si>
+  <si>
+    <t>https://www.alteo.fr/</t>
+  </si>
+  <si>
+    <t>Alteo</t>
+  </si>
+  <si>
+    <t>http://www.lafabriquedunet.fr</t>
+  </si>
+  <si>
+    <t>La Fabrique du Net</t>
+  </si>
+  <si>
+    <t>01 85 08 37 48</t>
+  </si>
+  <si>
+    <t>http://www.sofracs.com/</t>
+  </si>
+  <si>
+    <t>Sofracs</t>
+  </si>
+  <si>
+    <t>01.43.79.86.30</t>
+  </si>
+  <si>
+    <t>01 55 25 49 90</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0#&quot; &quot;##&quot; &quot;##&quot; &quot;##&quot; &quot;##"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -233,17 +359,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0#&quot; &quot;##&quot; &quot;##&quot; &quot;##&quot; &quot;##"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -254,6 +389,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau22" displayName="Tableau22" ref="A1:J1048576" totalsRowShown="0">
+  <autoFilter ref="A1:J1048576"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Entreprise"/>
+    <tableColumn id="2" name="Site"/>
+    <tableColumn id="3" name="Domaine"/>
+    <tableColumn id="4" name="1er contact"/>
+    <tableColumn id="9" name="Méthode"/>
+    <tableColumn id="5" name="nom"/>
+    <tableColumn id="6" name="Call 1 "/>
+    <tableColumn id="7" name="résultat"/>
+    <tableColumn id="8" name="Annonce"/>
+    <tableColumn id="10" name="tel" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:I1048576" totalsRowShown="0">
   <autoFilter ref="A1:I1048576"/>
   <tableColumns count="9">
@@ -534,9 +688,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="2">
+        <v>140445280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="J11" s="2">
+        <v>972377333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1">
+        <v>42460</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="1">
+        <v>42460</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>